<commit_message>
Correzione files Eliot 3.0
Correzione Files Eliot 3.0 per errato test 191
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_3.0/20.15.04/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_3.0/20.15.04/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DOCUMENTI\CDA_FSE2.0\AccreditamentoFSE20\pubblicati\Eliot_3.0\20.15.04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1DCE82-875B-44F1-B8B8-BE92B94C6B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ADB1AF-44A7-4971-AE85-D5E985EA8CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,12 +600,6 @@
     <t>subject_application_version:20.15.04</t>
   </si>
   <si>
-    <t>05bf2feb0003c4da</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.150.4.4.ea153a088f048ed3d94cbaba83d766ce99b4440e7e56122de8f8aa35e8f51266.aeace24a17^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
     <t>4092306d21627ba6</t>
   </si>
   <si>
@@ -694,9 +688,6 @@
   </si>
   <si>
     <t>2023-03-13T14:39:36Z</t>
-  </si>
-  <si>
-    <t>2023-03-13T09:54:28Z</t>
   </si>
   <si>
     <t>2023-03-14T10:00:13Z</t>
@@ -829,6 +820,15 @@
   </si>
   <si>
     <t>Applicativo Trasfusionale, il test OK è il 191.</t>
+  </si>
+  <si>
+    <t>2023-04-06T16:27:30Z</t>
+  </si>
+  <si>
+    <t>638dba87f774d117</t>
+  </si>
+  <si>
+    <t>"2.16.840.1.113883.2.9.2.150.4.4.5e98dd32b2085f500d10e6cffefbaf2768b4c48208dc004af8b895bda82eba43.a238558202^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
 </sst>
 </file>
@@ -1286,28 +1286,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1332,11 +1310,33 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2784,10 +2784,10 @@
   <dimension ref="A1:T823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,14 +2828,14 @@
       <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -2853,14 +2853,14 @@
       <c r="T2" s="32"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="48"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2878,12 +2878,12 @@
       <c r="T3" s="32"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -2902,12 +2902,12 @@
       <c r="T4" s="32"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="48"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -2925,8 +2925,8 @@
       <c r="T5" s="32"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -3044,35 +3044,35 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47">
+      <c r="A10" s="35">
         <v>1</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52" t="s">
+      <c r="D10" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
+      <c r="K10" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="21"/>
@@ -3080,35 +3080,35 @@
       <c r="T10" s="19"/>
     </row>
     <row r="11" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47">
+      <c r="A11" s="35">
         <v>2</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52" t="s">
+      <c r="D11" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="K11" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="42"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="21"/>
@@ -3116,35 +3116,35 @@
       <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47">
+      <c r="A12" s="35">
         <v>3</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52" t="s">
+      <c r="D12" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="K12" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="42"/>
       <c r="P12" s="19"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="21"/>
@@ -3152,35 +3152,35 @@
       <c r="T12" s="19"/>
     </row>
     <row r="13" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47">
+      <c r="A13" s="35">
         <v>4</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="E13" s="49" t="s">
+      <c r="D13" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="K13" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="21"/>
@@ -3188,35 +3188,35 @@
       <c r="T13" s="19"/>
     </row>
     <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47">
+      <c r="A14" s="35">
         <v>5</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="E14" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52" t="s">
+      <c r="D14" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
+      <c r="K14" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="21"/>
@@ -3243,13 +3243,13 @@
         <v>44998</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>33</v>
@@ -3262,13 +3262,13 @@
         <v>33</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
@@ -3297,13 +3297,13 @@
         <v>44998</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>33</v>
@@ -3316,13 +3316,13 @@
         <v>33</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20"/>
@@ -3351,7 +3351,7 @@
         <v>44998</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -3362,7 +3362,7 @@
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
       <c r="P17" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="20" t="s">
@@ -3393,13 +3393,13 @@
         <v>44998</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>33</v>
@@ -3412,13 +3412,13 @@
         <v>33</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
@@ -3427,7 +3427,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>53</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>76</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -3485,13 +3485,13 @@
         <v>44998</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>33</v>
@@ -3504,13 +3504,13 @@
         <v>33</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
@@ -3539,13 +3539,13 @@
         <v>44998</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>33</v>
@@ -3558,13 +3558,13 @@
         <v>33</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>76</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
@@ -3593,13 +3593,13 @@
         <v>44998</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>33</v>
@@ -3612,13 +3612,13 @@
         <v>33</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O22" s="19" t="s">
         <v>76</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
@@ -3647,13 +3647,13 @@
         <v>44999</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>33</v>
@@ -3666,13 +3666,13 @@
         <v>33</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
@@ -3701,13 +3701,13 @@
         <v>44999</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>33</v>
@@ -3720,13 +3720,13 @@
         <v>33</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
@@ -3755,13 +3755,13 @@
         <v>44999</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>33</v>
@@ -3774,13 +3774,13 @@
         <v>33</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
@@ -3809,13 +3809,13 @@
         <v>44999</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>33</v>
@@ -3828,13 +3828,13 @@
         <v>33</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
@@ -3863,13 +3863,13 @@
         <v>44999</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>33</v>
@@ -3882,13 +3882,13 @@
         <v>33</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
@@ -3917,13 +3917,13 @@
         <v>44999</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>33</v>
@@ -3936,13 +3936,13 @@
         <v>33</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O28" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="20"/>
@@ -3968,16 +3968,16 @@
         <v>84</v>
       </c>
       <c r="F29" s="17">
-        <v>44998</v>
+        <v>45022</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>111</v>
+        <v>181</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>33</v>
@@ -19965,15 +19965,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -19982,6 +19973,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20004,14 +20004,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -20028,6 +20020,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Rieseguiti test 28 e 36
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_3.0/20.15.04/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_3.0/20.15.04/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DOCUMENTI\CDA_FSE2.0\AccreditamentoFSE20\pubblicati\Eliot_3.0\20.15.04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ADB1AF-44A7-4971-AE85-D5E985EA8CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A10857-039B-43F5-9751-A54A69ACFA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,22 +600,10 @@
     <t>subject_application_version:20.15.04</t>
   </si>
   <si>
-    <t>4092306d21627ba6</t>
-  </si>
-  <si>
     <t>"UNKNOWN_WORKFLOW_ID"</t>
   </si>
   <si>
     <t>Errore di collegamento al gateway</t>
-  </si>
-  <si>
-    <t>Il mancato collegamento comporta la mancata validazione, verrà registrato l'errore ":"Campo token JWT non valido.","detail":"Il campo purpose_of_use non è valorizzato","status":403"  sul registro degli eventi dell'applicativo, l'utente è avvisato con un apposito messaggio di cortesia. La Validazione verrà ritentata in automatico appena ripristinato l'errore.</t>
-  </si>
-  <si>
-    <t>2013-03-13T10:35:08Z</t>
-  </si>
-  <si>
-    <t>5635b1831bbc534f</t>
   </si>
   <si>
     <t>Il mancato collegamento comporta la mancata validazione, verrà registrato l'errore ""Il campo action_id non è corretto","status":403, " sul registro degli eventi dell'applicativo, l'utente è avvisato con un apposito messaggio di cortesia. La velidazione verrà riprovata in automatico appena ripristinato l'errore.</t>
@@ -670,9 +658,6 @@
   </si>
   <si>
     <t>Dovranno essere corretti i dati anagrafici direttamente dal Personale e poi rieseguita la validazione. L'errore completo è memorizzato e visibile nel registro degli eventi: "Errore semantico.","detail":"[ERRORE-15| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']","status":422,"instance":"/validation/error"</t>
-  </si>
-  <si>
-    <t>2023-03-13T10:13:37Z</t>
   </si>
   <si>
     <t>2023-03-13T10:48:08Z</t>
@@ -829,6 +814,21 @@
   </si>
   <si>
     <t>"2.16.840.1.113883.2.9.2.150.4.4.5e98dd32b2085f500d10e6cffefbaf2768b4c48208dc004af8b895bda82eba43.a238558202^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>dfede93fbf7738bc</t>
+  </si>
+  <si>
+    <t>Il mancato collegamento comporta la mancata validazione, verrà registrato l'errore ":"title":"Campo token JWT non valido.","detail":"Il campo purpose_of_use non è valorizzato","status":403,"instance":"/jwt-mandatory-field-missing"  sul registro degli eventi dell'applicativo, l'utente è avvisato con un apposito messaggio di cortesia. La Validazione verrà ritentata in automatico appena ripristinato l'errore.</t>
+  </si>
+  <si>
+    <t>2023-04-26T11:53:19Z</t>
+  </si>
+  <si>
+    <t>f206f9776730ff96</t>
+  </si>
+  <si>
+    <t>2023-04-26T12:04:27Z</t>
   </si>
 </sst>
 </file>
@@ -2784,10 +2784,10 @@
   <dimension ref="A1:T823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3054,10 +3054,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="39"/>
@@ -3067,7 +3067,7 @@
         <v>76</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="40"/>
@@ -3090,10 +3090,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="39"/>
@@ -3103,7 +3103,7 @@
         <v>76</v>
       </c>
       <c r="K11" s="44" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L11" s="40"/>
       <c r="M11" s="40"/>
@@ -3126,10 +3126,10 @@
         <v>26</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
@@ -3139,7 +3139,7 @@
         <v>76</v>
       </c>
       <c r="K12" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
@@ -3162,10 +3162,10 @@
         <v>26</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="39"/>
@@ -3175,7 +3175,7 @@
         <v>76</v>
       </c>
       <c r="K13" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
@@ -3198,10 +3198,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="39"/>
@@ -3211,7 +3211,7 @@
         <v>76</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
@@ -3223,7 +3223,7 @@
       <c r="S14" s="31"/>
       <c r="T14" s="19"/>
     </row>
-    <row r="15" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>28</v>
       </c>
@@ -3240,16 +3240,16 @@
         <v>104</v>
       </c>
       <c r="F15" s="17">
-        <v>44998</v>
+        <v>45042</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="H15" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>110</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>33</v>
@@ -3262,13 +3262,13 @@
         <v>33</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
@@ -3294,16 +3294,16 @@
         <v>105</v>
       </c>
       <c r="F16" s="17">
-        <v>44998</v>
+        <v>45042</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>33</v>
@@ -3316,13 +3316,13 @@
         <v>33</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20"/>
@@ -3351,7 +3351,7 @@
         <v>44998</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -3362,7 +3362,7 @@
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
       <c r="P17" s="19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="20" t="s">
@@ -3393,13 +3393,13 @@
         <v>44998</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>33</v>
@@ -3412,13 +3412,13 @@
         <v>33</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
@@ -3451,7 +3451,7 @@
         <v>76</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -3485,13 +3485,13 @@
         <v>44998</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>33</v>
@@ -3504,13 +3504,13 @@
         <v>33</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
@@ -3539,13 +3539,13 @@
         <v>44998</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>33</v>
@@ -3558,13 +3558,13 @@
         <v>33</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>76</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
@@ -3593,13 +3593,13 @@
         <v>44998</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>33</v>
@@ -3612,13 +3612,13 @@
         <v>33</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="O22" s="19" t="s">
         <v>76</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
@@ -3647,13 +3647,13 @@
         <v>44999</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>33</v>
@@ -3666,13 +3666,13 @@
         <v>33</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
@@ -3701,13 +3701,13 @@
         <v>44999</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>33</v>
@@ -3720,13 +3720,13 @@
         <v>33</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P24" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
@@ -3755,13 +3755,13 @@
         <v>44999</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>33</v>
@@ -3774,13 +3774,13 @@
         <v>33</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
@@ -3809,13 +3809,13 @@
         <v>44999</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>33</v>
@@ -3828,13 +3828,13 @@
         <v>33</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
@@ -3863,13 +3863,13 @@
         <v>44999</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>33</v>
@@ -3882,13 +3882,13 @@
         <v>33</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
@@ -3917,13 +3917,13 @@
         <v>44999</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>33</v>
@@ -3936,13 +3936,13 @@
         <v>33</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="O28" s="19" t="s">
         <v>33</v>
       </c>
       <c r="P28" s="19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="20"/>
@@ -3971,13 +3971,13 @@
         <v>45022</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>33</v>
@@ -19965,6 +19965,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -19973,15 +19982,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20004,6 +20004,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -20020,14 +20028,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>